<commit_message>
Working IEEE reader API.
</commit_message>
<xml_diff>
--- a/simplepower/models/grid_model_data/OPF_grid1.xlsx
+++ b/simplepower/models/grid_model_data/OPF_grid1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uisn-my.sharepoint.com/personal/emelf_usn_no/Documents/PhD - SysOpt/Python Work/Custom Modules/simplepower/simplepower/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uisn-my.sharepoint.com/personal/emelf_usn_no/Documents/PhD - SysOpt/Python Work/Custom Modules/simplepower/simplepower/models/grid_model_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="419" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C781EEDB-C6E2-4712-88CE-3218F676AE37}"/>
+  <xr:revisionPtr revIDLastSave="425" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0E6A5E6-C2C7-4FE3-AD8C-A039F91FB0A6}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>name</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>G1</t>
+  </si>
+  <si>
+    <t>s_base_mva</t>
+  </si>
+  <si>
+    <t>g_shunt_pu</t>
+  </si>
+  <si>
+    <t>b_shunt_pu</t>
   </si>
 </sst>
 </file>
@@ -719,10 +728,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF97191-B8C8-4B12-8921-F601069D1D4E}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,38 +739,62 @@
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -853,7 +886,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>